<commit_message>
Update as of Nov 19, 2024
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\geoscan_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\geoscan_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED0CD56-DCDA-47D2-AE11-16FE91C14377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97D582DB-4A03-4D2D-9BA2-93F8CB1B972A}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Student ID</t>
   </si>
@@ -62,50 +61,17 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
-    <t>123-456-7890</t>
-  </si>
-  <si>
-    <t>123 Elm Street</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>jane.smith@example.com</t>
-  </si>
-  <si>
-    <t>987-654-3210</t>
-  </si>
-  <si>
-    <t>456 Oak Avenue</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>alice.johnson@example.com</t>
-  </si>
-  <si>
-    <t>555-123-4567</t>
-  </si>
-  <si>
-    <t>789 Pine Road</t>
+    <t>johndoe@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +83,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,10 +113,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -150,8 +125,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -483,24 +462,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CCFEF1-6E74-4E8E-9CCC-983EDD897356}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,9 +499,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" customHeight="1">
       <c r="A2" s="2">
-        <v>5789457</v>
+        <v>1231234</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -530,57 +509,49 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>123123123</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" customHeight="1">
       <c r="A3" s="2">
-        <v>5789458</v>
+        <v>123123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>123123123</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>5789450</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
+    <row r="4" spans="1:6" ht="18" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>